<commit_message>
Actualize diagrama de paginas
</commit_message>
<xml_diff>
--- a/app/paginas.xlsx
+++ b/app/paginas.xlsx
@@ -468,58 +468,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="62 Conector curvado"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="19" idx="3"/>
-          <a:endCxn id="34" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7315199" y="1676400"/>
-          <a:ext cx="209551" cy="1781176"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -109090"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -4554,6 +4502,647 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="136" name="135 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9839325" y="2457449"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/consumibles/registar</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="137" name="136 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8086725" y="2457449"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/consumibles/ver/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="138" name="137 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11925300" y="2628899"/>
+          <a:ext cx="1752600" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/consumibles/editar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="139" name="138 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="37" idx="3"/>
+          <a:endCxn id="137" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7372350" y="2571750"/>
+          <a:ext cx="714375" cy="19049"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="140" name="139 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="137" idx="3"/>
+          <a:endCxn id="136" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9563100" y="2590799"/>
+          <a:ext cx="276225" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="141" name="140 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="136" idx="3"/>
+          <a:endCxn id="161" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11315700" y="2114550"/>
+          <a:ext cx="1019175" cy="476249"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="141 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="136" idx="3"/>
+          <a:endCxn id="138" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11315700" y="2590799"/>
+          <a:ext cx="609600" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442914</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>376238</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="143" name="142 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="137" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="10467976" y="357188"/>
+          <a:ext cx="457199" cy="3743324"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="144" name="143 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="137" idx="2"/>
+          <a:endCxn id="138" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="10727531" y="821530"/>
+          <a:ext cx="171450" cy="3976687"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 233333"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442913</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="147" name="146 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="138" idx="0"/>
+          <a:endCxn id="137" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="10727532" y="554830"/>
+          <a:ext cx="171450" cy="3976687"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 233333"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442914</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="159" name="158 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="161" idx="2"/>
+          <a:endCxn id="137" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10889458" y="183356"/>
+          <a:ext cx="209549" cy="4338637"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="161" name="160 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12334875" y="1981200"/>
+          <a:ext cx="1657350" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/consumibles/borar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4848,8 +5437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Diagrama de paginas actualizado
</commit_message>
<xml_diff>
--- a/app/paginas.xlsx
+++ b/app/paginas.xlsx
@@ -126,16 +126,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170090</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>73479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -144,7 +144,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5857875" y="1543050"/>
+          <a:off x="6266090" y="2930979"/>
           <a:ext cx="1666875" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -183,16 +183,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187779</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130628</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -201,7 +201,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5848350" y="3324226"/>
+          <a:off x="6283779" y="3419476"/>
           <a:ext cx="1466849" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -241,15 +241,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:colOff>585108</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>83003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:colOff>537483</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>159203</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -258,7 +258,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5867400" y="5400676"/>
+          <a:off x="5919108" y="16847003"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -297,15 +297,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>344261</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296636</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -315,7 +315,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5895975" y="2438400"/>
+          <a:off x="6440261" y="1676400"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -411,16 +411,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>187779</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>17689</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>73479</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -429,7 +429,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8324850" y="4229100"/>
+          <a:off x="12257314" y="3616779"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -468,16 +468,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>160564</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>187779</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>103413</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>73479</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -486,7 +486,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5848350" y="4324351"/>
+          <a:off x="6256564" y="3997779"/>
           <a:ext cx="1466849" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -753,16 +753,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>186418</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>138793</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -771,7 +771,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10201275" y="4210050"/>
+          <a:off x="14664418" y="3652157"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -810,16 +810,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130628</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -831,8 +831,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7315199" y="3457576"/>
-          <a:ext cx="1009651" cy="904874"/>
+          <a:off x="7750628" y="3552826"/>
+          <a:ext cx="4506686" cy="197303"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -862,16 +862,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>17689</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>186418</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -882,9 +882,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9801225" y="4343400"/>
-          <a:ext cx="400050" cy="19050"/>
+        <a:xfrm>
+          <a:off x="13733689" y="3750129"/>
+          <a:ext cx="930729" cy="35378"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -914,16 +914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>103413</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>73479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>41502</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -934,15 +934,12 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315199" y="4457701"/>
-          <a:ext cx="1747839" cy="38099"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector4">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 28883"/>
-            <a:gd name="adj2" fmla="val 700016"/>
-          </a:avLst>
+        <a:xfrm flipV="1">
+          <a:off x="7723413" y="3883479"/>
+          <a:ext cx="5272089" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -3487,84 +3484,188 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170089</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="27 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="19" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943600" y="642937"/>
+          <a:ext cx="322489" cy="2421391"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -70886"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>344261</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="145" name="144 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="37" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943601" y="642938"/>
+          <a:ext cx="496660" cy="1166812"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -46027"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>609601</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="27 Conector curvado"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="1"/>
-          <a:endCxn id="19" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5857875" y="642938"/>
-          <a:ext cx="85726" cy="1033462"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 366664"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187779</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="145 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="34" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943601" y="642938"/>
+          <a:ext cx="340178" cy="2909888"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -67200"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>609601</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="145" name="144 Conector curvado"/>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>160563</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>130628</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="148" name="147 Conector curvado"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="1"/>
-          <a:endCxn id="37" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5895975" y="642938"/>
-          <a:ext cx="47626" cy="1928812"/>
+          <a:endCxn id="68" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943600" y="642937"/>
+          <a:ext cx="312963" cy="3488191"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 579990"/>
+            <a:gd name="adj1" fmla="val -73044"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3591,119 +3692,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>514351</xdr:colOff>
+      <xdr:colOff>585109</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>609602</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="146" name="145 Conector curvado"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="1"/>
-          <a:endCxn id="34" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5848351" y="642938"/>
-          <a:ext cx="95251" cy="2814638"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 339997"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>609602</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="148" name="147 Conector curvado"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="1"/>
-          <a:endCxn id="68" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5848351" y="642937"/>
-          <a:ext cx="95251" cy="3814763"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 339997"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>609602</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>25852</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3715,12 +3712,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5867401" y="642938"/>
-          <a:ext cx="76201" cy="4891088"/>
+          <a:off x="5919109" y="642937"/>
+          <a:ext cx="24493" cy="16337415"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 399996"/>
+            <a:gd name="adj1" fmla="val 1033328"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4506,16 +4503,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42182</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>62592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:colOff>756557</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>138792</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4524,7 +4521,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9839325" y="2457449"/>
+          <a:off x="9948182" y="2539092"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4564,15 +4561,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>643618</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>117018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>595993</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>2718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4581,7 +4578,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8086725" y="2457449"/>
+          <a:off x="8263618" y="2403018"/>
           <a:ext cx="1476375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4621,15 +4618,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>753836</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>84363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>220436</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>160563</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4638,7 +4635,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11925300" y="2628899"/>
+          <a:off x="12183836" y="2560863"/>
           <a:ext cx="1752600" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4677,16 +4674,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296636</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>643618</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>59868</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4698,8 +4695,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7372350" y="2571750"/>
-          <a:ext cx="714375" cy="19049"/>
+          <a:off x="7916636" y="1809750"/>
+          <a:ext cx="346982" cy="726618"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -4730,15 +4727,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>595993</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>126999</xdr:rowOff>
+      <xdr:rowOff>59868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42182</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5442</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4750,8 +4747,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9563100" y="2590799"/>
-          <a:ext cx="276225" cy="12700"/>
+          <a:off x="9739993" y="2536368"/>
+          <a:ext cx="208189" cy="136074"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -4782,15 +4779,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:colOff>756557</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5442</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4802,8 +4799,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11315700" y="2114550"/>
-          <a:ext cx="1019175" cy="476249"/>
+          <a:off x="11424557" y="2114550"/>
+          <a:ext cx="910318" cy="557892"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -4834,15 +4831,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>756557</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>753836</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>27213</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4854,8 +4851,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11315700" y="2590799"/>
-          <a:ext cx="609600" cy="171450"/>
+          <a:off x="11424557" y="2672442"/>
+          <a:ext cx="759279" cy="21771"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -4886,30 +4883,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>442914</xdr:colOff>
+      <xdr:colOff>619806</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>376238</xdr:colOff>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>117018</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="143" name="142 Conector curvado"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="137" idx="0"/>
+          <a:endCxn id="161" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="10467976" y="357188"/>
-          <a:ext cx="457199" cy="3743324"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector2">
-          <a:avLst/>
+          <a:off x="10871769" y="111237"/>
+          <a:ext cx="421818" cy="4161744"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 154194"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -4935,15 +4935,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
+      <xdr:colOff>619807</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>2717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>106137</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>160562</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4955,12 +4955,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="10727531" y="821530"/>
-          <a:ext cx="171450" cy="3976687"/>
+          <a:off x="10952049" y="719475"/>
+          <a:ext cx="157845" cy="4058330"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 233333"/>
+            <a:gd name="adj1" fmla="val 244826"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4987,15 +4987,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>442913</xdr:colOff>
+      <xdr:colOff>619807</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:rowOff>117018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>106137</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>84363</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5007,12 +5007,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="10727532" y="554830"/>
-          <a:ext cx="171450" cy="3976687"/>
+          <a:off x="10952049" y="452776"/>
+          <a:ext cx="157845" cy="4058330"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 233333"/>
+            <a:gd name="adj1" fmla="val 244826"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -5039,15 +5039,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>442914</xdr:colOff>
+      <xdr:colOff>619806</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>117018</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5059,8 +5059,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="10889458" y="183356"/>
-          <a:ext cx="209549" cy="4338637"/>
+          <a:off x="11005119" y="244587"/>
+          <a:ext cx="155118" cy="4161744"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -5143,6 +5143,1510 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>612321</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>551089</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>134710</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="162" name="161 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5946321" y="13811250"/>
+          <a:ext cx="1462768" cy="229960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/compras/</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>612321</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>19730</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="163" name="162 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="162" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943601" y="642938"/>
+          <a:ext cx="2720" cy="13283292"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -8404412"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>710293</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>662668</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="200" name="199 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9854293" y="13615307"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/compras/registar</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>481693</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>434068</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="201" name="200 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8101693" y="13615307"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/compras/ver/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>415018</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="202" name="201 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11845018" y="13158107"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/compras/borar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>300718</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="203" name="202 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11778343" y="13805807"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/compras/editar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>548368</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>481693</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="204" name="203 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="201" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7406368" y="13748657"/>
+          <a:ext cx="695325" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>434068</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>710293</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="205" name="204 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="201" idx="3"/>
+          <a:endCxn id="200" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9578068" y="13748657"/>
+          <a:ext cx="276225" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>662668</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>146957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>415018</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="206" name="205 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="200" idx="3"/>
+          <a:endCxn id="202" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11330668" y="13291457"/>
+          <a:ext cx="514350" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>662668</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="207" name="206 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="200" idx="3"/>
+          <a:endCxn id="203" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11330668" y="13748657"/>
+          <a:ext cx="447675" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457880</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>13608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>391205</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>89808</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="208" name="207 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="201" idx="0"/>
+          <a:endCxn id="202" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="10482943" y="11515045"/>
+          <a:ext cx="457200" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 150000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457881</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>324531</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="209" name="208 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="201" idx="2"/>
+          <a:endCxn id="203" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="10582956" y="12138932"/>
+          <a:ext cx="190500" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 220000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457881</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>324531</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="210" name="209 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="203" idx="0"/>
+          <a:endCxn id="201" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="10582956" y="11872232"/>
+          <a:ext cx="190500" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 160000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457881</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>89808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>391206</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>89808</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="211" name="210 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="202" idx="2"/>
+          <a:endCxn id="201" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10616294" y="11648395"/>
+          <a:ext cx="190500" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29999"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>706210</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>658585</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="212" name="211 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9850210" y="16676914"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/ventas/registar</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>477610</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>429985</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="213" name="212 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8097610" y="16676914"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/ventas/ver/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>410935</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>363310</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="214" name="213 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11840935" y="16219714"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/ventas/borar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>344260</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>296635</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="215" name="214 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11774260" y="16867414"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/ventas/editar/$id</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>477610</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="216" name="215 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="213" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7402285" y="16810264"/>
+          <a:ext cx="695325" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>429985</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>706210</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>58964</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="217" name="216 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="213" idx="3"/>
+          <a:endCxn id="212" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9573985" y="16810264"/>
+          <a:ext cx="276225" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>658585</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>160564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>410935</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="218" name="217 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="212" idx="3"/>
+          <a:endCxn id="214" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11326585" y="16353064"/>
+          <a:ext cx="514350" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>658585</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>344260</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="219" name="218 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="212" idx="3"/>
+          <a:endCxn id="215" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11326585" y="16810264"/>
+          <a:ext cx="447675" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>453797</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>387122</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="220" name="219 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="213" idx="0"/>
+          <a:endCxn id="214" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="10478860" y="14576652"/>
+          <a:ext cx="457200" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 150000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>453798</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>320448</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="221" name="220 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="213" idx="2"/>
+          <a:endCxn id="215" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="10578873" y="15200539"/>
+          <a:ext cx="190500" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 220000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>453798</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>320448</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="222" name="221 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="215" idx="0"/>
+          <a:endCxn id="213" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="10578873" y="14933839"/>
+          <a:ext cx="190500" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 160000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>453798</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>387123</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="223" name="222 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="214" idx="2"/>
+          <a:endCxn id="213" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10612211" y="14710002"/>
+          <a:ext cx="190500" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29999"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>696686</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>153760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>649061</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>39460</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="224" name="223 Rectángulo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6030686" y="18632260"/>
+          <a:ext cx="1476375" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>/archivos/</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>696685</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>96610</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="225" name="224 Conector curvado"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="224" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="5943600" y="642938"/>
+          <a:ext cx="87085" cy="18122672"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -403128"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5437,8 +6941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>